<commit_message>
doc. updates - gantt stuff
</commit_message>
<xml_diff>
--- a/Gantt chart.xlsx
+++ b/Gantt chart.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25629"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harri\Desktop\Submit\2022\S2\SoftTech\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC02D53D-F129-4C2C-972B-8726DE1C68CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A58F4133-076B-44CD-8613-AD6DA9B76EFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -628,6 +628,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="12">
       <alignment vertical="center"/>
     </xf>
@@ -639,42 +675,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -699,26 +699,6 @@
     <cellStyle name="Title" xfId="8" builtinId="15" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="9">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </right>
-        <bottom style="thin">
-          <color theme="7"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -830,6 +810,26 @@
         <bottom style="thin">
           <color theme="0"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="7"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
   </dxfs>
@@ -1078,8 +1078,8 @@
   </sheetPr>
   <dimension ref="B1:BO39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="U8" sqref="U8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1106,13 +1106,13 @@
       <c r="G1" s="12"/>
     </row>
     <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
       <c r="G2" s="5" t="s">
         <v>13</v>
       </c>
@@ -1120,37 +1120,37 @@
         <v>1</v>
       </c>
       <c r="J2" s="15"/>
-      <c r="K2" s="29" t="s">
+      <c r="K2" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="31"/>
+      <c r="L2" s="26"/>
+      <c r="M2" s="26"/>
+      <c r="N2" s="26"/>
+      <c r="O2" s="27"/>
       <c r="P2" s="16"/>
-      <c r="Q2" s="29" t="s">
+      <c r="Q2" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="R2" s="32"/>
-      <c r="S2" s="32"/>
-      <c r="T2" s="31"/>
+      <c r="R2" s="28"/>
+      <c r="S2" s="28"/>
+      <c r="T2" s="27"/>
       <c r="U2" s="17"/>
-      <c r="V2" s="33" t="s">
+      <c r="V2" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="W2" s="34"/>
-      <c r="X2" s="34"/>
-      <c r="Y2" s="35"/>
+      <c r="W2" s="30"/>
+      <c r="X2" s="30"/>
+      <c r="Y2" s="31"/>
       <c r="Z2" s="18"/>
-      <c r="AA2" s="36" t="s">
+      <c r="AA2" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="AB2" s="37"/>
-      <c r="AC2" s="37"/>
-      <c r="AD2" s="37"/>
-      <c r="AE2" s="37"/>
-      <c r="AF2" s="37"/>
-      <c r="AG2" s="38"/>
+      <c r="AB2" s="33"/>
+      <c r="AC2" s="33"/>
+      <c r="AD2" s="33"/>
+      <c r="AE2" s="33"/>
+      <c r="AF2" s="33"/>
+      <c r="AG2" s="34"/>
       <c r="AH2" s="19"/>
       <c r="AI2" s="21" t="s">
         <v>12</v>
@@ -1164,22 +1164,22 @@
       <c r="AP2" s="22"/>
     </row>
     <row r="3" spans="2:67" s="11" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="26" t="s">
+      <c r="B3" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="26" t="s">
+      <c r="D3" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="26" t="s">
+      <c r="E3" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="26" t="s">
+      <c r="F3" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="28" t="s">
+      <c r="G3" s="23" t="s">
         <v>18</v>
       </c>
       <c r="H3" s="20" t="s">
@@ -1206,12 +1206,12 @@
       <c r="AA3" s="10"/>
     </row>
     <row r="4" spans="2:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="25"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
       <c r="H4" s="3">
         <v>1</v>
       </c>
@@ -1638,15 +1638,19 @@
         <v>44</v>
       </c>
       <c r="C17" s="7">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D17" s="7">
-        <v>1</v>
-      </c>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
+        <v>4</v>
+      </c>
+      <c r="E17" s="7">
+        <v>24</v>
+      </c>
+      <c r="F17" s="7">
+        <v>4</v>
+      </c>
       <c r="G17" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -1659,10 +1663,14 @@
       <c r="D18" s="7">
         <v>1</v>
       </c>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
+      <c r="E18" s="7">
+        <v>28</v>
+      </c>
+      <c r="F18" s="7">
+        <v>1</v>
+      </c>
       <c r="G18" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -1675,10 +1683,14 @@
       <c r="D19" s="7">
         <v>15</v>
       </c>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
+      <c r="E19" s="7">
+        <v>10</v>
+      </c>
+      <c r="F19" s="7">
+        <v>17</v>
+      </c>
       <c r="G19" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -1691,10 +1703,14 @@
       <c r="D20" s="7">
         <v>11</v>
       </c>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
+      <c r="E20" s="7">
+        <v>10</v>
+      </c>
+      <c r="F20" s="7">
+        <v>15</v>
+      </c>
       <c r="G20" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -1707,10 +1723,14 @@
       <c r="D21" s="7">
         <v>4</v>
       </c>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
+      <c r="E21" s="7">
+        <v>21</v>
+      </c>
+      <c r="F21" s="7">
+        <v>4</v>
+      </c>
       <c r="G21" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -1723,10 +1743,14 @@
       <c r="D22" s="7">
         <v>3</v>
       </c>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
+      <c r="E22" s="7">
+        <v>21</v>
+      </c>
+      <c r="F22" s="7">
+        <v>7</v>
+      </c>
       <c r="G22" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -1935,47 +1959,47 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="K2:O2"/>
-    <mergeCell ref="Q2:T2"/>
-    <mergeCell ref="V2:Y2"/>
-    <mergeCell ref="AA2:AG2"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="K2:O2"/>
+    <mergeCell ref="Q2:T2"/>
+    <mergeCell ref="V2:Y2"/>
+    <mergeCell ref="AA2:AG2"/>
   </mergeCells>
   <phoneticPr fontId="14" type="noConversion"/>
   <conditionalFormatting sqref="H5:BO39">
-    <cfRule type="expression" dxfId="8" priority="1">
+    <cfRule type="expression" dxfId="7" priority="1">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="3">
+    <cfRule type="expression" dxfId="6" priority="3">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="4">
+    <cfRule type="expression" dxfId="5" priority="4">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="5">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="6">
+    <cfRule type="expression" dxfId="3" priority="6">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="7">
+    <cfRule type="expression" dxfId="2" priority="7">
       <formula>H$4=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="11">
+    <cfRule type="expression" dxfId="1" priority="11">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="12">
+    <cfRule type="expression" dxfId="0" priority="12">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:BO4">
-    <cfRule type="expression" dxfId="0" priority="8">
+    <cfRule type="expression" dxfId="8" priority="8">
       <formula>H$4=period_selected</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>